<commit_message>
GL Update - Translist Report
Controller - Adjust query and cell value inputs
Index - Add checkbox for summary only (in progress)
excel template - adjusted column width.
</commit_message>
<xml_diff>
--- a/public/excel_templates/transaction-list-report-template-lo.xlsx
+++ b/public/excel_templates/transaction-list-report-template-lo.xlsx
@@ -26,28 +26,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Acc. Code</t>
+  </si>
+  <si>
+    <t>Cost Ctr.</t>
+  </si>
+  <si>
+    <t>Account Title</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
     <t>Unlimited Network of Opportunities International Corp.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>TIN: 006-505-014 VAT</t>
-  </si>
-  <si>
-    <t>Acc. Code</t>
-  </si>
-  <si>
-    <t>Cost Ctr.</t>
-  </si>
-  <si>
-    <t>Account Title</t>
-  </si>
-  <si>
-    <t>Debit</t>
-  </si>
-  <si>
-    <t>Credit</t>
   </si>
 </sst>
 </file>
@@ -387,31 +387,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -420,31 +423,27 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>